<commit_message>
feedback pass 1 complete
</commit_message>
<xml_diff>
--- a/docs/price_calculator_template.xlsx
+++ b/docs/price_calculator_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28117"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28122"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usilr\Desktop\GourmetPro\calculator\price-structure-calculator\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BAA9486-8508-4690-8E5D-9022F6FB7BAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1298EF0C-C3DF-4571-AA31-5972B1E13E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,7 +96,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +129,13 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -487,7 +494,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -590,6 +597,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -854,7 +864,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z28" sqref="Z28"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -924,30 +934,30 @@
     <row r="3" spans="1:26" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
-      <c r="U3" s="14"/>
-      <c r="V3" s="14"/>
-      <c r="W3" s="14"/>
-      <c r="X3" s="14"/>
-      <c r="Y3" s="14"/>
-      <c r="Z3" s="14"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="50"/>
+      <c r="N3" s="50"/>
+      <c r="O3" s="50"/>
+      <c r="P3" s="50"/>
+      <c r="Q3" s="50"/>
+      <c r="R3" s="50"/>
+      <c r="S3" s="50"/>
+      <c r="T3" s="50"/>
+      <c r="U3" s="50"/>
+      <c r="V3" s="50"/>
+      <c r="W3" s="50"/>
+      <c r="X3" s="50"/>
+      <c r="Y3" s="50"/>
+      <c r="Z3" s="50"/>
     </row>
     <row r="4" spans="1:26" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="16"/>

</xml_diff>

<commit_message>
excel template updated, various CSS updates
</commit_message>
<xml_diff>
--- a/docs/price_calculator_template.xlsx
+++ b/docs/price_calculator_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usilr\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usilr\Desktop\GourmetPro\calculator\price-structure-calculator\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D32703-064B-41C6-97B7-FE41A29096FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA435415-48FA-46CE-B593-1AB12472CFD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Units Per Shipment</t>
   </si>
@@ -88,12 +88,24 @@
   <si>
     <t>Result</t>
   </si>
+  <si>
+    <t>Importer Amount</t>
+  </si>
+  <si>
+    <t>Product Price</t>
+  </si>
+  <si>
+    <t>Wholesaler Amount</t>
+  </si>
+  <si>
+    <t>Retailer Amount</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,6 +156,12 @@
     <font>
       <b/>
       <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -211,7 +229,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -321,22 +339,6 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -548,11 +550,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -571,8 +623,8 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -582,8 +634,8 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -598,73 +650,57 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -674,27 +710,76 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -956,10 +1041,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB1003"/>
+  <dimension ref="A1:AB1011"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1184,11 +1269,11 @@
       <c r="A8" s="45"/>
       <c r="B8" s="46"/>
       <c r="C8" s="48">
-        <f>IF(OR(ISBLANK(C6), ISBLANK(C7)), "", ROUND(C6 / (1 - C7/100), 0))</f>
-        <v>806</v>
+        <f>IF(OR(ISBLANK(C6), ISBLANK(C7)), "", ROUND(C6 / (1 - C7/100), 2))</f>
+        <v>806.45</v>
       </c>
       <c r="D8" s="48" t="str">
-        <f t="shared" ref="D8:Z8" si="0">IF(OR(ISBLANK(D6), ISBLANK(D7)), "", ROUND(D6 / (1 - D7/100), 0))</f>
+        <f t="shared" ref="D8:Z8" si="0">IF(OR(ISBLANK(D6), ISBLANK(D7)), "", ROUND(D6 / (1 - D7/100), 2))</f>
         <v/>
       </c>
       <c r="E8" s="48" t="str">
@@ -1378,15 +1463,15 @@
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="2">
-        <f>IF(OR(ISBLANK(C11), ISBLANK(C6), ISBLANK(C7), ISBLANK(C10)), "", ROUND((C6/(1-(C7/100))) + (C10/C11), 0))</f>
-        <v>807</v>
+        <f>IF(OR(ISBLANK(C11), ISBLANK(C6), ISBLANK(C7), ISBLANK(C10)), "", ROUND((C6/(1-(C7/100))) + (C10/C11), 2))</f>
+        <v>807.25</v>
       </c>
       <c r="D12" s="2" t="str">
-        <f>IF(OR(ISBLANK(D11), ISBLANK(D6), ISBLANK(D7), ISBLANK(D10)), "", ROUND((D6/(1-(D7/100))) + (D10/D11), 0))</f>
+        <f t="shared" ref="D12:Z12" si="1">IF(OR(ISBLANK(D11), ISBLANK(D6), ISBLANK(D7), ISBLANK(D10)), "", ROUND((D6/(1-(D7/100))) + (D10/D11), 2))</f>
         <v/>
       </c>
       <c r="E12" s="2" t="str">
-        <f t="shared" ref="E12:Z12" si="1">IF(OR(ISBLANK(E11), ISBLANK(E6), ISBLANK(E7), ISBLANK(E10)), "", ROUND((E6/(1-(E7/100))) + (E10/E11), 0))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F12" s="2" t="str">
@@ -1469,7 +1554,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="Z12" s="2" t="str">
+      <c r="Z12" s="68" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -1572,11 +1657,11 @@
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="2">
-        <f t="shared" ref="C16:Z16" si="2">IF(OR(ISBLANK(C12), ISBLANK(C14), ISBLANK(C15)), "", ROUND(C12 * (1 + C14/100) + C15, 0))</f>
-        <v>880</v>
+        <f>IF(OR(ISBLANK(C12), ISBLANK(C14), ISBLANK(C15)), "", ROUND(C12 * (1 + C14/100) + C15, 2))</f>
+        <v>879.9</v>
       </c>
       <c r="D16" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D16:Z16" si="2">IF(OR(ISBLANK(D12), ISBLANK(D14), ISBLANK(D15)), "", ROUND(D12 * (1 + D14/100) + D15, 2))</f>
         <v/>
       </c>
       <c r="E16" s="2" t="str">
@@ -1663,12 +1748,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="Z16" s="2" t="str">
+      <c r="Z16" s="68" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:26" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4"/>
       <c r="B17" s="19" t="s">
         <v>9</v>
@@ -1698,7 +1783,7 @@
       <c r="Y17" s="16"/>
       <c r="Z17" s="16"/>
     </row>
-    <row r="18" spans="1:28" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:26" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
       <c r="B18" s="12" t="s">
         <v>10</v>
@@ -1730,7 +1815,7 @@
       <c r="Y18" s="16"/>
       <c r="Z18" s="16"/>
     </row>
-    <row r="19" spans="1:28" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:26" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4"/>
       <c r="B19" s="12" t="s">
         <v>11</v>
@@ -1762,7 +1847,7 @@
       <c r="Y19" s="16"/>
       <c r="Z19" s="16"/>
     </row>
-    <row r="20" spans="1:28" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:26" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4"/>
       <c r="B20" s="12" t="s">
         <v>12</v>
@@ -1794,15 +1879,15 @@
       <c r="Y20" s="16"/>
       <c r="Z20" s="16"/>
     </row>
-    <row r="21" spans="1:28" s="3" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:26" s="3" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="2">
-        <f t="shared" ref="C21:Z21" si="3">IF(OR(ISBLANK(C16), ISBLANK(C18), ISBLANK(C19), ISBLANK(C20)), "", C16 + C18 + C19 + C20)</f>
-        <v>990</v>
+        <f>IF(OR(ISBLANK(C16), ISBLANK(C18), ISBLANK(C19), ISBLANK(C20)), "", ROUND(C16 + C18 + C19 + C20, 2))</f>
+        <v>989.9</v>
       </c>
       <c r="D21" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="D21:Z21" si="3">IF(OR(ISBLANK(D16), ISBLANK(D18), ISBLANK(D19), ISBLANK(D20)), "", ROUND(D16 + D18 + D19 + D20, 2))</f>
         <v/>
       </c>
       <c r="E21" s="2" t="str">
@@ -1889,12 +1974,12 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="Z21" s="2" t="str">
+      <c r="Z21" s="68" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:28" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:26" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4"/>
       <c r="B22" s="19"/>
       <c r="C22" s="20"/>
@@ -1922,579 +2007,1023 @@
       <c r="Y22" s="16"/>
       <c r="Z22" s="16"/>
     </row>
-    <row r="23" spans="1:28" s="28" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="50"/>
+    <row r="23" spans="1:26" s="75" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="69"/>
       <c r="B23" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="51">
+      <c r="C23" s="71">
         <v>30</v>
       </c>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="53"/>
-      <c r="G23" s="54"/>
-      <c r="H23" s="54"/>
-      <c r="I23" s="54"/>
-      <c r="J23" s="54"/>
-      <c r="K23" s="54"/>
-      <c r="L23" s="54"/>
-      <c r="M23" s="54"/>
-      <c r="N23" s="54"/>
-      <c r="O23" s="54"/>
-      <c r="P23" s="54"/>
-      <c r="Q23" s="54"/>
-      <c r="R23" s="54"/>
-      <c r="S23" s="54"/>
-      <c r="T23" s="54"/>
-      <c r="U23" s="54"/>
-      <c r="V23" s="54"/>
-      <c r="W23" s="54"/>
-      <c r="X23" s="54"/>
-      <c r="Y23" s="54"/>
-      <c r="Z23" s="54"/>
-    </row>
-    <row r="24" spans="1:28" s="28" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="50"/>
-      <c r="B24" s="70" t="s">
+      <c r="D23" s="72"/>
+      <c r="E23" s="72"/>
+      <c r="F23" s="73"/>
+      <c r="G23" s="74"/>
+      <c r="H23" s="74"/>
+      <c r="I23" s="74"/>
+      <c r="J23" s="74"/>
+      <c r="K23" s="74"/>
+      <c r="L23" s="74"/>
+      <c r="M23" s="74"/>
+      <c r="N23" s="74"/>
+      <c r="O23" s="74"/>
+      <c r="P23" s="74"/>
+      <c r="Q23" s="74"/>
+      <c r="R23" s="74"/>
+      <c r="S23" s="74"/>
+      <c r="T23" s="74"/>
+      <c r="U23" s="74"/>
+      <c r="V23" s="74"/>
+      <c r="W23" s="74"/>
+      <c r="X23" s="74"/>
+      <c r="Y23" s="74"/>
+      <c r="Z23" s="74"/>
+    </row>
+    <row r="24" spans="1:26" s="28" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="61"/>
+      <c r="B24" s="63" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="66">
+        <f>IF(OR(ISBLANK(C21), ISBLANK(C23)), "", ROUND(C21 / (1 - C23 / 100), 2))</f>
+        <v>1414.14</v>
+      </c>
+      <c r="D24" s="66" t="str">
+        <f t="shared" ref="D24:Z24" si="4">IF(OR(ISBLANK(D21), ISBLANK(D23)), "", ROUND(D21 / (1 - D23 / 100), 2))</f>
+        <v/>
+      </c>
+      <c r="E24" s="66" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F24" s="66" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="G24" s="66" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="H24" s="66" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="I24" s="66" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="J24" s="66" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K24" s="66" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L24" s="66" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M24" s="66" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="N24" s="66" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="O24" s="66" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="P24" s="66" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q24" s="66" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="R24" s="66" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S24" s="66" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="T24" s="66" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="U24" s="66" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="V24" s="66" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="W24" s="66" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="X24" s="66" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Y24" s="66" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Z24" s="82" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:26" s="79" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="76"/>
+      <c r="B25" s="77" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="78">
+        <f>IF(OR(C24="", C21=""), "", ROUND(C24 - C21, 2))</f>
+        <v>424.24</v>
+      </c>
+      <c r="D25" s="78" t="str">
+        <f t="shared" ref="D25:Z25" si="5">IF(OR(D24="", D21=""), "", ROUND(D24 - D21, 2))</f>
+        <v/>
+      </c>
+      <c r="E25" s="78" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F25" s="78" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="G25" s="78" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="H25" s="78" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="I25" s="78" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="J25" s="78" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="K25" s="78" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="L25" s="78" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M25" s="78" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N25" s="78" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O25" s="78" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="P25" s="78" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="Q25" s="78" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="R25" s="78" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="S25" s="78" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="T25" s="78" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="U25" s="78" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="V25" s="78" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="W25" s="78" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="X25" s="78" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="Y25" s="78" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="Z25" s="83" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:26" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="27"/>
+      <c r="B26" s="64"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="16"/>
+      <c r="O26" s="16"/>
+      <c r="P26" s="16"/>
+      <c r="Q26" s="16"/>
+      <c r="R26" s="16"/>
+      <c r="S26" s="16"/>
+      <c r="T26" s="16"/>
+      <c r="U26" s="16"/>
+      <c r="V26" s="16"/>
+      <c r="W26" s="16"/>
+      <c r="X26" s="16"/>
+      <c r="Y26" s="16"/>
+      <c r="Z26" s="16"/>
+    </row>
+    <row r="27" spans="1:26" s="75" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="69"/>
+      <c r="B27" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="51">
+      <c r="C27" s="71">
         <v>15</v>
       </c>
-      <c r="D24" s="52"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="53"/>
-      <c r="G24" s="54"/>
-      <c r="H24" s="54"/>
-      <c r="I24" s="54"/>
-      <c r="J24" s="54"/>
-      <c r="K24" s="54"/>
-      <c r="L24" s="54"/>
-      <c r="M24" s="54"/>
-      <c r="N24" s="54"/>
-      <c r="O24" s="54"/>
-      <c r="P24" s="54"/>
-      <c r="Q24" s="54"/>
-      <c r="R24" s="54"/>
-      <c r="S24" s="54"/>
-      <c r="T24" s="54"/>
-      <c r="U24" s="54"/>
-      <c r="V24" s="54"/>
-      <c r="W24" s="54"/>
-      <c r="X24" s="54"/>
-      <c r="Y24" s="54"/>
-      <c r="Z24" s="54"/>
-    </row>
-    <row r="25" spans="1:28" s="28" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="55"/>
-      <c r="B25" s="69" t="s">
+      <c r="D27" s="72"/>
+      <c r="E27" s="72"/>
+      <c r="F27" s="73"/>
+      <c r="G27" s="74"/>
+      <c r="H27" s="74"/>
+      <c r="I27" s="74"/>
+      <c r="J27" s="74"/>
+      <c r="K27" s="74"/>
+      <c r="L27" s="74"/>
+      <c r="M27" s="74"/>
+      <c r="N27" s="74"/>
+      <c r="O27" s="74"/>
+      <c r="P27" s="74"/>
+      <c r="Q27" s="74"/>
+      <c r="R27" s="74"/>
+      <c r="S27" s="74"/>
+      <c r="T27" s="74"/>
+      <c r="U27" s="74"/>
+      <c r="V27" s="74"/>
+      <c r="W27" s="74"/>
+      <c r="X27" s="74"/>
+      <c r="Y27" s="74"/>
+      <c r="Z27" s="74"/>
+    </row>
+    <row r="28" spans="1:26" s="28" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="61"/>
+      <c r="B28" s="63" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="62">
+        <f>IF(OR(ISBLANK(C24), ISBLANK(C27)), "", ROUND(C24 / (1 - C27 / 100), 2))</f>
+        <v>1663.69</v>
+      </c>
+      <c r="D28" s="62" t="str">
+        <f t="shared" ref="D28:Z28" si="6">IF(OR(ISBLANK(D24), ISBLANK(D27)), "", ROUND(D24 / (1 - D27 / 100), 2))</f>
+        <v/>
+      </c>
+      <c r="E28" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="F28" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="G28" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="H28" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I28" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="J28" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="K28" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="L28" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="M28" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="N28" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O28" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="P28" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q28" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="R28" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="S28" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="T28" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="U28" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="V28" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="W28" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="X28" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Y28" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Z28" s="67" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:26" s="79" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="76"/>
+      <c r="B29" s="77" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="80">
+        <f>IF(OR(C28="", C24=""), "", ROUND(C28 - C24, 2))</f>
+        <v>249.55</v>
+      </c>
+      <c r="D29" s="80" t="str">
+        <f t="shared" ref="D29:Z29" si="7">IF(OR(D28="", D24=""), "", ROUND(D28 - D24, 2))</f>
+        <v/>
+      </c>
+      <c r="E29" s="80" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="F29" s="80" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="G29" s="80" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="H29" s="80" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="I29" s="80" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="J29" s="80" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="K29" s="80" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="L29" s="80" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="M29" s="80" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="N29" s="80" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="O29" s="80" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P29" s="80" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="Q29" s="80" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="R29" s="80" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="S29" s="80" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="T29" s="80" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="U29" s="80" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="V29" s="80" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="W29" s="80" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="X29" s="80" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="Y29" s="80" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="Z29" s="81" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:26" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="27"/>
+      <c r="B30" s="65"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="16"/>
+      <c r="O30" s="16"/>
+      <c r="P30" s="16"/>
+      <c r="Q30" s="16"/>
+      <c r="R30" s="16"/>
+      <c r="S30" s="16"/>
+      <c r="T30" s="16"/>
+      <c r="U30" s="16"/>
+      <c r="V30" s="16"/>
+      <c r="W30" s="16"/>
+      <c r="X30" s="16"/>
+      <c r="Y30" s="16"/>
+      <c r="Z30" s="16"/>
+    </row>
+    <row r="31" spans="1:26" s="75" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="69"/>
+      <c r="B31" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="56">
+      <c r="C31" s="71">
         <v>25</v>
       </c>
-      <c r="D25" s="57"/>
-      <c r="E25" s="57"/>
-      <c r="F25" s="53"/>
-      <c r="G25" s="54"/>
-      <c r="H25" s="54"/>
-      <c r="I25" s="54"/>
-      <c r="J25" s="54"/>
-      <c r="K25" s="54"/>
-      <c r="L25" s="54"/>
-      <c r="M25" s="54"/>
-      <c r="N25" s="54"/>
-      <c r="O25" s="54"/>
-      <c r="P25" s="54"/>
-      <c r="Q25" s="54"/>
-      <c r="R25" s="54"/>
-      <c r="S25" s="54"/>
-      <c r="T25" s="54"/>
-      <c r="U25" s="54"/>
-      <c r="V25" s="54"/>
-      <c r="W25" s="54"/>
-      <c r="X25" s="54"/>
-      <c r="Y25" s="54"/>
-      <c r="Z25" s="54"/>
-    </row>
-    <row r="26" spans="1:28" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="27"/>
-      <c r="B26" s="36"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="65"/>
-      <c r="F26" s="66"/>
-      <c r="G26" s="66"/>
-      <c r="H26" s="66"/>
-      <c r="I26" s="66"/>
-      <c r="J26" s="66"/>
-      <c r="K26" s="66"/>
-      <c r="L26" s="66"/>
-      <c r="M26" s="66"/>
-      <c r="N26" s="66"/>
-      <c r="O26" s="66"/>
-      <c r="P26" s="66"/>
-      <c r="Q26" s="66"/>
-      <c r="R26" s="66"/>
-      <c r="S26" s="66"/>
-      <c r="T26" s="66"/>
-      <c r="U26" s="66"/>
-      <c r="V26" s="66"/>
-      <c r="W26" s="66"/>
-      <c r="X26" s="66"/>
-      <c r="Y26" s="66"/>
-      <c r="Z26" s="15"/>
-    </row>
-    <row r="27" spans="1:28" s="3" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="58"/>
-      <c r="B27" s="59" t="s">
+      <c r="D31" s="72"/>
+      <c r="E31" s="72"/>
+      <c r="F31" s="73"/>
+      <c r="G31" s="74"/>
+      <c r="H31" s="74"/>
+      <c r="I31" s="74"/>
+      <c r="J31" s="74"/>
+      <c r="K31" s="74"/>
+      <c r="L31" s="74"/>
+      <c r="M31" s="74"/>
+      <c r="N31" s="74"/>
+      <c r="O31" s="74"/>
+      <c r="P31" s="74"/>
+      <c r="Q31" s="74"/>
+      <c r="R31" s="74"/>
+      <c r="S31" s="74"/>
+      <c r="T31" s="74"/>
+      <c r="U31" s="74"/>
+      <c r="V31" s="74"/>
+      <c r="W31" s="74"/>
+      <c r="X31" s="74"/>
+      <c r="Y31" s="74"/>
+      <c r="Z31" s="74"/>
+    </row>
+    <row r="32" spans="1:26" s="28" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="61"/>
+      <c r="B32" s="63" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="62">
+        <f>IF(OR(ISBLANK(C28), ISBLANK(C31)), "", ROUND(C28 / (1 - C31 / 100), 2))</f>
+        <v>2218.25</v>
+      </c>
+      <c r="D32" s="62" t="str">
+        <f t="shared" ref="D32:Z32" si="8">IF(OR(ISBLANK(D28), ISBLANK(D31)), "", ROUND(D28 / (1 - D31 / 100), 2))</f>
+        <v/>
+      </c>
+      <c r="E32" s="62" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="F32" s="62" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="G32" s="62" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="H32" s="62" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="I32" s="62" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="J32" s="62" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="K32" s="62" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="L32" s="62" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="M32" s="62" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="N32" s="62" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O32" s="62" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="P32" s="62" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="Q32" s="62" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="R32" s="62" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="S32" s="62" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="T32" s="62" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="U32" s="62" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="V32" s="62" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="W32" s="62" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="X32" s="62" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="Y32" s="62" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="Z32" s="67" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:28" s="79" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="76"/>
+      <c r="B33" s="77" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="80">
+        <f>IF(OR(C32="", C28=""), "", ROUND(C32 - C28, 2))</f>
+        <v>554.55999999999995</v>
+      </c>
+      <c r="D33" s="80" t="str">
+        <f t="shared" ref="D33:Z33" si="9">IF(OR(D32="", D28=""), "", ROUND(D32 - D28, 2))</f>
+        <v/>
+      </c>
+      <c r="E33" s="80" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="F33" s="80" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="G33" s="80" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="H33" s="80" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="I33" s="80" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="J33" s="80" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="K33" s="80" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L33" s="80" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="M33" s="80" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="N33" s="80" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="O33" s="80" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="P33" s="80" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="Q33" s="80" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="R33" s="80" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="S33" s="80" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="T33" s="80" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="U33" s="80" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="V33" s="80" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="W33" s="80" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="X33" s="80" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="Y33" s="80" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="Z33" s="81" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:28" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="27"/>
+      <c r="B34" s="36"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="58"/>
+      <c r="G34" s="58"/>
+      <c r="H34" s="58"/>
+      <c r="I34" s="58"/>
+      <c r="J34" s="58"/>
+      <c r="K34" s="58"/>
+      <c r="L34" s="58"/>
+      <c r="M34" s="58"/>
+      <c r="N34" s="58"/>
+      <c r="O34" s="58"/>
+      <c r="P34" s="58"/>
+      <c r="Q34" s="58"/>
+      <c r="R34" s="58"/>
+      <c r="S34" s="58"/>
+      <c r="T34" s="58"/>
+      <c r="U34" s="58"/>
+      <c r="V34" s="58"/>
+      <c r="W34" s="58"/>
+      <c r="X34" s="58"/>
+      <c r="Y34" s="58"/>
+      <c r="Z34" s="15"/>
+    </row>
+    <row r="35" spans="1:28" s="3" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="50"/>
+      <c r="B35" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="60" t="str">
-        <f>IF(C4&lt;&gt;"", C4 &amp; " " &amp; IF(OR(ISBLANK(C21), ISBLANK(C23), ISBLANK(C24), ISBLANK(C25)), "", ROUND(C21 / (1 - C23/100) / (1 - C24/100) / (1 - C25/100), 0)), "")</f>
-        <v>JPY 2218</v>
-      </c>
-      <c r="D27" s="60" t="str">
-        <f t="shared" ref="D27:Z27" si="4">IF(D4&lt;&gt;"", D4 &amp; " " &amp; IF(OR(ISBLANK(D21), ISBLANK(D23), ISBLANK(D24), ISBLANK(D25)), "", ROUND(D21 / (1 - D23/100) / (1 - D24/100) / (1 - D25/100), 0)), "")</f>
-        <v/>
-      </c>
-      <c r="E27" s="60" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="F27" s="60" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="G27" s="60" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="H27" s="60" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="I27" s="60" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="J27" s="60" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="K27" s="60" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="L27" s="60" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="M27" s="60" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="N27" s="60" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O27" s="60" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="P27" s="60" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="Q27" s="60" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="R27" s="60" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="S27" s="60" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="T27" s="60" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="U27" s="60" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="V27" s="60" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="W27" s="60" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="X27" s="60" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="Y27" s="60" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="Z27" s="60" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="AA27" s="67"/>
-      <c r="AB27" s="68"/>
-    </row>
-    <row r="28" spans="1:28" s="44" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="62"/>
-      <c r="B28" s="63"/>
-      <c r="C28" s="64"/>
-      <c r="D28" s="64"/>
-      <c r="E28" s="64"/>
-      <c r="F28" s="64"/>
-      <c r="G28" s="64"/>
-      <c r="H28" s="64"/>
-      <c r="I28" s="64"/>
-      <c r="J28" s="64"/>
-      <c r="K28" s="64"/>
-      <c r="L28" s="64"/>
-      <c r="M28" s="64"/>
-      <c r="N28" s="64"/>
-      <c r="O28" s="64"/>
-      <c r="P28" s="64"/>
-      <c r="Q28" s="64"/>
-      <c r="R28" s="64"/>
-      <c r="S28" s="64"/>
-      <c r="T28" s="64"/>
-      <c r="U28" s="64"/>
-      <c r="V28" s="64"/>
-      <c r="W28" s="64"/>
-      <c r="X28" s="64"/>
-      <c r="Y28" s="64"/>
-      <c r="Z28" s="64"/>
-      <c r="AA28" s="32"/>
-      <c r="AB28" s="32"/>
-    </row>
-    <row r="29" spans="1:28" s="32" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="27"/>
-      <c r="B29" s="61"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
-      <c r="K29" s="27"/>
-      <c r="L29" s="27"/>
-      <c r="M29" s="27"/>
-      <c r="N29" s="27"/>
-      <c r="O29" s="27"/>
-      <c r="P29" s="27"/>
-      <c r="Q29" s="27"/>
-      <c r="R29" s="27"/>
-      <c r="S29" s="27"/>
-      <c r="T29" s="27"/>
-      <c r="U29" s="27"/>
-      <c r="V29" s="27"/>
-      <c r="W29" s="27"/>
-      <c r="X29" s="27"/>
-      <c r="Y29" s="27"/>
-      <c r="Z29" s="27"/>
-    </row>
-    <row r="30" spans="1:28" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="24"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
-      <c r="K30" s="24"/>
-      <c r="L30" s="24"/>
-      <c r="M30" s="24"/>
-      <c r="N30" s="24"/>
-      <c r="O30" s="24"/>
-      <c r="P30" s="24"/>
-      <c r="Q30" s="24"/>
-      <c r="R30" s="24"/>
-      <c r="S30" s="24"/>
-      <c r="T30" s="24"/>
-      <c r="U30" s="24"/>
-      <c r="V30" s="24"/>
-      <c r="W30" s="24"/>
-      <c r="X30" s="24"/>
-      <c r="Y30" s="24"/>
-      <c r="Z30" s="24"/>
-    </row>
-    <row r="31" spans="1:28" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="25"/>
-      <c r="B31" s="26"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="25"/>
-      <c r="K31" s="25"/>
-      <c r="L31" s="25"/>
-      <c r="M31" s="25"/>
-      <c r="N31" s="25"/>
-      <c r="O31" s="25"/>
-      <c r="P31" s="25"/>
-      <c r="Q31" s="25"/>
-      <c r="R31" s="25"/>
-      <c r="S31" s="25"/>
-      <c r="T31" s="25"/>
-      <c r="U31" s="25"/>
-      <c r="V31" s="25"/>
-      <c r="W31" s="25"/>
-      <c r="X31" s="25"/>
-      <c r="Y31" s="25"/>
-      <c r="Z31" s="25"/>
-    </row>
-    <row r="32" spans="1:28" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="4"/>
-      <c r="B32" s="23"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-      <c r="P32" s="4"/>
-      <c r="Q32" s="4"/>
-      <c r="R32" s="4"/>
-      <c r="S32" s="4"/>
-      <c r="T32" s="4"/>
-      <c r="U32" s="4"/>
-      <c r="V32" s="4"/>
-      <c r="W32" s="4"/>
-      <c r="X32" s="4"/>
-      <c r="Y32" s="4"/>
-      <c r="Z32" s="4"/>
-    </row>
-    <row r="33" spans="1:26" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="4"/>
-      <c r="B33" s="23"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4"/>
-      <c r="Q33" s="4"/>
-      <c r="R33" s="4"/>
-      <c r="S33" s="4"/>
-      <c r="T33" s="4"/>
-      <c r="U33" s="4"/>
-      <c r="V33" s="4"/>
-      <c r="W33" s="4"/>
-      <c r="X33" s="4"/>
-      <c r="Y33" s="4"/>
-      <c r="Z33" s="4"/>
-    </row>
-    <row r="34" spans="1:26" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
-      <c r="O34" s="4"/>
-      <c r="P34" s="4"/>
-      <c r="Q34" s="4"/>
-      <c r="R34" s="4"/>
-      <c r="S34" s="4"/>
-      <c r="T34" s="4"/>
-      <c r="U34" s="4"/>
-      <c r="V34" s="4"/>
-      <c r="W34" s="4"/>
-      <c r="X34" s="4"/>
-      <c r="Y34" s="4"/>
-      <c r="Z34" s="4"/>
-    </row>
-    <row r="35" spans="1:26" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-      <c r="P35" s="4"/>
-      <c r="Q35" s="4"/>
-      <c r="R35" s="4"/>
-      <c r="S35" s="4"/>
-      <c r="T35" s="4"/>
-      <c r="U35" s="4"/>
-      <c r="V35" s="4"/>
-      <c r="W35" s="4"/>
-      <c r="X35" s="4"/>
-      <c r="Y35" s="4"/>
-      <c r="Z35" s="4"/>
-    </row>
-    <row r="36" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
-      <c r="P36" s="4"/>
-      <c r="Q36" s="4"/>
-      <c r="R36" s="4"/>
-      <c r="S36" s="4"/>
-      <c r="T36" s="4"/>
-      <c r="U36" s="4"/>
-      <c r="V36" s="4"/>
-      <c r="W36" s="4"/>
-      <c r="X36" s="4"/>
-      <c r="Y36" s="4"/>
-      <c r="Z36" s="4"/>
-    </row>
-    <row r="37" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="27"/>
-      <c r="D37" s="27"/>
-      <c r="E37" s="27"/>
+      <c r="C35" s="52" t="str">
+        <f>IF(C4&lt;&gt;"", C4 &amp; " " &amp; IF(C32&lt;&gt;"", C32, ""), "")</f>
+        <v>JPY 2218.25</v>
+      </c>
+      <c r="D35" s="52" t="str">
+        <f t="shared" ref="D35:Z35" si="10">IF(D4&lt;&gt;"", D4 &amp; " " &amp; IF(D32&lt;&gt;"", D32, ""), "")</f>
+        <v/>
+      </c>
+      <c r="E35" s="52" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="F35" s="52" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="G35" s="52" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="H35" s="52" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="I35" s="52" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="J35" s="52" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="K35" s="52" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="L35" s="52" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="M35" s="52" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="N35" s="52" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="O35" s="52" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="P35" s="52" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="Q35" s="52" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="R35" s="52" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="S35" s="52" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="T35" s="52" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="U35" s="52" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="V35" s="52" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="W35" s="52" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="X35" s="52" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="Y35" s="52" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="Z35" s="52" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="AA35" s="59"/>
+      <c r="AB35" s="60"/>
+    </row>
+    <row r="36" spans="1:28" s="44" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="54"/>
+      <c r="B36" s="55"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="56"/>
+      <c r="F36" s="56"/>
+      <c r="G36" s="56"/>
+      <c r="H36" s="56"/>
+      <c r="I36" s="56"/>
+      <c r="J36" s="56"/>
+      <c r="K36" s="56"/>
+      <c r="L36" s="56"/>
+      <c r="M36" s="56"/>
+      <c r="N36" s="56"/>
+      <c r="O36" s="56"/>
+      <c r="P36" s="56"/>
+      <c r="Q36" s="56"/>
+      <c r="R36" s="56"/>
+      <c r="S36" s="56"/>
+      <c r="T36" s="56"/>
+      <c r="U36" s="56"/>
+      <c r="V36" s="56"/>
+      <c r="W36" s="56"/>
+      <c r="X36" s="56"/>
+      <c r="Y36" s="56"/>
+      <c r="Z36" s="56"/>
+      <c r="AA36" s="32"/>
+      <c r="AB36" s="32"/>
+    </row>
+    <row r="37" spans="1:28" s="32" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="27"/>
+      <c r="B37" s="53"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="29"/>
       <c r="F37" s="27"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
-      <c r="N37" s="4"/>
-      <c r="O37" s="4"/>
-      <c r="P37" s="4"/>
-      <c r="Q37" s="4"/>
-      <c r="R37" s="4"/>
-      <c r="S37" s="4"/>
-      <c r="T37" s="4"/>
-      <c r="U37" s="4"/>
-      <c r="V37" s="4"/>
-      <c r="W37" s="4"/>
-      <c r="X37" s="4"/>
-      <c r="Y37" s="4"/>
-      <c r="Z37" s="4"/>
-    </row>
-    <row r="38" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="27"/>
-      <c r="D38" s="27"/>
-      <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
-      <c r="N38" s="4"/>
-      <c r="O38" s="4"/>
-      <c r="P38" s="4"/>
-      <c r="Q38" s="4"/>
-      <c r="R38" s="4"/>
-      <c r="S38" s="4"/>
-      <c r="T38" s="4"/>
-      <c r="U38" s="4"/>
-      <c r="V38" s="4"/>
-      <c r="W38" s="4"/>
-      <c r="X38" s="4"/>
-      <c r="Y38" s="4"/>
-      <c r="Z38" s="4"/>
-    </row>
-    <row r="39" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="27"/>
-      <c r="D39" s="27"/>
-      <c r="E39" s="27"/>
-      <c r="F39" s="27"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
-      <c r="N39" s="4"/>
-      <c r="O39" s="4"/>
-      <c r="P39" s="4"/>
-      <c r="Q39" s="4"/>
-      <c r="R39" s="4"/>
-      <c r="S39" s="4"/>
-      <c r="T39" s="4"/>
-      <c r="U39" s="4"/>
-      <c r="V39" s="4"/>
-      <c r="W39" s="4"/>
-      <c r="X39" s="4"/>
-      <c r="Y39" s="4"/>
-      <c r="Z39" s="4"/>
-    </row>
-    <row r="40" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G37" s="27"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="27"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="27"/>
+      <c r="L37" s="27"/>
+      <c r="M37" s="27"/>
+      <c r="N37" s="27"/>
+      <c r="O37" s="27"/>
+      <c r="P37" s="27"/>
+      <c r="Q37" s="27"/>
+      <c r="R37" s="27"/>
+      <c r="S37" s="27"/>
+      <c r="T37" s="27"/>
+      <c r="U37" s="27"/>
+      <c r="V37" s="27"/>
+      <c r="W37" s="27"/>
+      <c r="X37" s="27"/>
+      <c r="Y37" s="27"/>
+      <c r="Z37" s="27"/>
+    </row>
+    <row r="38" spans="1:28" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="24"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="24"/>
+      <c r="J38" s="24"/>
+      <c r="K38" s="24"/>
+      <c r="L38" s="24"/>
+      <c r="M38" s="24"/>
+      <c r="N38" s="24"/>
+      <c r="O38" s="24"/>
+      <c r="P38" s="24"/>
+      <c r="Q38" s="24"/>
+      <c r="R38" s="24"/>
+      <c r="S38" s="24"/>
+      <c r="T38" s="24"/>
+      <c r="U38" s="24"/>
+      <c r="V38" s="24"/>
+      <c r="W38" s="24"/>
+      <c r="X38" s="24"/>
+      <c r="Y38" s="24"/>
+      <c r="Z38" s="24"/>
+    </row>
+    <row r="39" spans="1:28" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="25"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="25"/>
+      <c r="K39" s="25"/>
+      <c r="L39" s="25"/>
+      <c r="M39" s="25"/>
+      <c r="N39" s="25"/>
+      <c r="O39" s="25"/>
+      <c r="P39" s="25"/>
+      <c r="Q39" s="25"/>
+      <c r="R39" s="25"/>
+      <c r="S39" s="25"/>
+      <c r="T39" s="25"/>
+      <c r="U39" s="25"/>
+      <c r="V39" s="25"/>
+      <c r="W39" s="25"/>
+      <c r="X39" s="25"/>
+      <c r="Y39" s="25"/>
+      <c r="Z39" s="25"/>
+    </row>
+    <row r="40" spans="1:28" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="4"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="27"/>
-      <c r="D40" s="27"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="4"/>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
@@ -2516,12 +3045,12 @@
       <c r="Y40" s="4"/>
       <c r="Z40" s="4"/>
     </row>
-    <row r="41" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:28" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="27"/>
-      <c r="D41" s="27"/>
-      <c r="E41" s="27"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="29"/>
       <c r="F41" s="27"/>
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
@@ -2544,7 +3073,7 @@
       <c r="Y41" s="4"/>
       <c r="Z41" s="4"/>
     </row>
-    <row r="42" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:28" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="27"/>
@@ -2572,7 +3101,7 @@
       <c r="Y42" s="4"/>
       <c r="Z42" s="4"/>
     </row>
-    <row r="43" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:28" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="27"/>
@@ -2600,7 +3129,7 @@
       <c r="Y43" s="4"/>
       <c r="Z43" s="4"/>
     </row>
-    <row r="44" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="27"/>
@@ -2628,7 +3157,7 @@
       <c r="Y44" s="4"/>
       <c r="Z44" s="4"/>
     </row>
-    <row r="45" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="27"/>
@@ -2656,7 +3185,7 @@
       <c r="Y45" s="4"/>
       <c r="Z45" s="4"/>
     </row>
-    <row r="46" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="27"/>
@@ -2684,7 +3213,7 @@
       <c r="Y46" s="4"/>
       <c r="Z46" s="4"/>
     </row>
-    <row r="47" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="27"/>
@@ -2712,7 +3241,7 @@
       <c r="Y47" s="4"/>
       <c r="Z47" s="4"/>
     </row>
-    <row r="48" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="27"/>
@@ -2993,116 +3522,300 @@
       <c r="Z57" s="4"/>
     </row>
     <row r="58" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C58" s="31"/>
-      <c r="D58" s="31"/>
-      <c r="E58" s="32"/>
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="27"/>
+      <c r="D58" s="27"/>
+      <c r="E58" s="27"/>
+      <c r="F58" s="27"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="4"/>
+      <c r="K58" s="4"/>
+      <c r="L58" s="4"/>
+      <c r="M58" s="4"/>
+      <c r="N58" s="4"/>
+      <c r="O58" s="4"/>
+      <c r="P58" s="4"/>
+      <c r="Q58" s="4"/>
+      <c r="R58" s="4"/>
+      <c r="S58" s="4"/>
+      <c r="T58" s="4"/>
+      <c r="U58" s="4"/>
+      <c r="V58" s="4"/>
+      <c r="W58" s="4"/>
+      <c r="X58" s="4"/>
+      <c r="Y58" s="4"/>
+      <c r="Z58" s="4"/>
     </row>
     <row r="59" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C59" s="31"/>
-      <c r="D59" s="31"/>
-      <c r="E59" s="32"/>
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="27"/>
+      <c r="D59" s="27"/>
+      <c r="E59" s="27"/>
+      <c r="F59" s="27"/>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="4"/>
+      <c r="J59" s="4"/>
+      <c r="K59" s="4"/>
+      <c r="L59" s="4"/>
+      <c r="M59" s="4"/>
+      <c r="N59" s="4"/>
+      <c r="O59" s="4"/>
+      <c r="P59" s="4"/>
+      <c r="Q59" s="4"/>
+      <c r="R59" s="4"/>
+      <c r="S59" s="4"/>
+      <c r="T59" s="4"/>
+      <c r="U59" s="4"/>
+      <c r="V59" s="4"/>
+      <c r="W59" s="4"/>
+      <c r="X59" s="4"/>
+      <c r="Y59" s="4"/>
+      <c r="Z59" s="4"/>
     </row>
     <row r="60" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C60" s="31"/>
-      <c r="D60" s="31"/>
-      <c r="E60" s="32"/>
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="27"/>
+      <c r="D60" s="27"/>
+      <c r="E60" s="27"/>
+      <c r="F60" s="27"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="4"/>
+      <c r="K60" s="4"/>
+      <c r="L60" s="4"/>
+      <c r="M60" s="4"/>
+      <c r="N60" s="4"/>
+      <c r="O60" s="4"/>
+      <c r="P60" s="4"/>
+      <c r="Q60" s="4"/>
+      <c r="R60" s="4"/>
+      <c r="S60" s="4"/>
+      <c r="T60" s="4"/>
+      <c r="U60" s="4"/>
+      <c r="V60" s="4"/>
+      <c r="W60" s="4"/>
+      <c r="X60" s="4"/>
+      <c r="Y60" s="4"/>
+      <c r="Z60" s="4"/>
     </row>
     <row r="61" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C61" s="31"/>
-      <c r="D61" s="31"/>
-      <c r="E61" s="32"/>
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="27"/>
+      <c r="D61" s="27"/>
+      <c r="E61" s="27"/>
+      <c r="F61" s="27"/>
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
+      <c r="J61" s="4"/>
+      <c r="K61" s="4"/>
+      <c r="L61" s="4"/>
+      <c r="M61" s="4"/>
+      <c r="N61" s="4"/>
+      <c r="O61" s="4"/>
+      <c r="P61" s="4"/>
+      <c r="Q61" s="4"/>
+      <c r="R61" s="4"/>
+      <c r="S61" s="4"/>
+      <c r="T61" s="4"/>
+      <c r="U61" s="4"/>
+      <c r="V61" s="4"/>
+      <c r="W61" s="4"/>
+      <c r="X61" s="4"/>
+      <c r="Y61" s="4"/>
+      <c r="Z61" s="4"/>
     </row>
     <row r="62" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C62" s="31"/>
-      <c r="D62" s="31"/>
-      <c r="E62" s="32"/>
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="27"/>
+      <c r="D62" s="27"/>
+      <c r="E62" s="27"/>
+      <c r="F62" s="27"/>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
+      <c r="J62" s="4"/>
+      <c r="K62" s="4"/>
+      <c r="L62" s="4"/>
+      <c r="M62" s="4"/>
+      <c r="N62" s="4"/>
+      <c r="O62" s="4"/>
+      <c r="P62" s="4"/>
+      <c r="Q62" s="4"/>
+      <c r="R62" s="4"/>
+      <c r="S62" s="4"/>
+      <c r="T62" s="4"/>
+      <c r="U62" s="4"/>
+      <c r="V62" s="4"/>
+      <c r="W62" s="4"/>
+      <c r="X62" s="4"/>
+      <c r="Y62" s="4"/>
+      <c r="Z62" s="4"/>
     </row>
     <row r="63" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C63" s="31"/>
-      <c r="D63" s="31"/>
-      <c r="E63" s="32"/>
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="27"/>
+      <c r="D63" s="27"/>
+      <c r="E63" s="27"/>
+      <c r="F63" s="27"/>
+      <c r="G63" s="4"/>
+      <c r="H63" s="4"/>
+      <c r="I63" s="4"/>
+      <c r="J63" s="4"/>
+      <c r="K63" s="4"/>
+      <c r="L63" s="4"/>
+      <c r="M63" s="4"/>
+      <c r="N63" s="4"/>
+      <c r="O63" s="4"/>
+      <c r="P63" s="4"/>
+      <c r="Q63" s="4"/>
+      <c r="R63" s="4"/>
+      <c r="S63" s="4"/>
+      <c r="T63" s="4"/>
+      <c r="U63" s="4"/>
+      <c r="V63" s="4"/>
+      <c r="W63" s="4"/>
+      <c r="X63" s="4"/>
+      <c r="Y63" s="4"/>
+      <c r="Z63" s="4"/>
     </row>
     <row r="64" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C64" s="31"/>
-      <c r="D64" s="31"/>
-      <c r="E64" s="32"/>
-    </row>
-    <row r="65" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C65" s="31"/>
-      <c r="D65" s="31"/>
-      <c r="E65" s="32"/>
-    </row>
-    <row r="66" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="27"/>
+      <c r="D64" s="27"/>
+      <c r="E64" s="27"/>
+      <c r="F64" s="27"/>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
+      <c r="I64" s="4"/>
+      <c r="J64" s="4"/>
+      <c r="K64" s="4"/>
+      <c r="L64" s="4"/>
+      <c r="M64" s="4"/>
+      <c r="N64" s="4"/>
+      <c r="O64" s="4"/>
+      <c r="P64" s="4"/>
+      <c r="Q64" s="4"/>
+      <c r="R64" s="4"/>
+      <c r="S64" s="4"/>
+      <c r="T64" s="4"/>
+      <c r="U64" s="4"/>
+      <c r="V64" s="4"/>
+      <c r="W64" s="4"/>
+      <c r="X64" s="4"/>
+      <c r="Y64" s="4"/>
+      <c r="Z64" s="4"/>
+    </row>
+    <row r="65" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="4"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="27"/>
+      <c r="D65" s="27"/>
+      <c r="E65" s="27"/>
+      <c r="F65" s="27"/>
+      <c r="G65" s="4"/>
+      <c r="H65" s="4"/>
+      <c r="I65" s="4"/>
+      <c r="J65" s="4"/>
+      <c r="K65" s="4"/>
+      <c r="L65" s="4"/>
+      <c r="M65" s="4"/>
+      <c r="N65" s="4"/>
+      <c r="O65" s="4"/>
+      <c r="P65" s="4"/>
+      <c r="Q65" s="4"/>
+      <c r="R65" s="4"/>
+      <c r="S65" s="4"/>
+      <c r="T65" s="4"/>
+      <c r="U65" s="4"/>
+      <c r="V65" s="4"/>
+      <c r="W65" s="4"/>
+      <c r="X65" s="4"/>
+      <c r="Y65" s="4"/>
+      <c r="Z65" s="4"/>
+    </row>
+    <row r="66" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C66" s="31"/>
       <c r="D66" s="31"/>
       <c r="E66" s="32"/>
     </row>
-    <row r="67" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C67" s="31"/>
       <c r="D67" s="31"/>
       <c r="E67" s="32"/>
     </row>
-    <row r="68" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C68" s="31"/>
       <c r="D68" s="31"/>
       <c r="E68" s="32"/>
     </row>
-    <row r="69" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C69" s="31"/>
       <c r="D69" s="31"/>
       <c r="E69" s="32"/>
     </row>
-    <row r="70" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C70" s="31"/>
       <c r="D70" s="31"/>
       <c r="E70" s="32"/>
     </row>
-    <row r="71" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C71" s="31"/>
       <c r="D71" s="31"/>
       <c r="E71" s="32"/>
     </row>
-    <row r="72" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C72" s="31"/>
       <c r="D72" s="31"/>
       <c r="E72" s="32"/>
     </row>
-    <row r="73" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C73" s="31"/>
       <c r="D73" s="31"/>
       <c r="E73" s="32"/>
     </row>
-    <row r="74" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C74" s="31"/>
       <c r="D74" s="31"/>
       <c r="E74" s="32"/>
     </row>
-    <row r="75" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C75" s="31"/>
       <c r="D75" s="31"/>
       <c r="E75" s="32"/>
     </row>
-    <row r="76" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C76" s="31"/>
       <c r="D76" s="31"/>
       <c r="E76" s="32"/>
     </row>
-    <row r="77" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C77" s="31"/>
       <c r="D77" s="31"/>
       <c r="E77" s="32"/>
     </row>
-    <row r="78" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C78" s="31"/>
       <c r="D78" s="31"/>
       <c r="E78" s="32"/>
     </row>
-    <row r="79" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C79" s="31"/>
       <c r="D79" s="31"/>
       <c r="E79" s="32"/>
     </row>
-    <row r="80" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C80" s="31"/>
       <c r="D80" s="31"/>
       <c r="E80" s="32"/>
@@ -7721,6 +8434,46 @@
       <c r="C1003" s="31"/>
       <c r="D1003" s="31"/>
       <c r="E1003" s="32"/>
+    </row>
+    <row r="1004" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C1004" s="31"/>
+      <c r="D1004" s="31"/>
+      <c r="E1004" s="32"/>
+    </row>
+    <row r="1005" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C1005" s="31"/>
+      <c r="D1005" s="31"/>
+      <c r="E1005" s="32"/>
+    </row>
+    <row r="1006" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C1006" s="31"/>
+      <c r="D1006" s="31"/>
+      <c r="E1006" s="32"/>
+    </row>
+    <row r="1007" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C1007" s="31"/>
+      <c r="D1007" s="31"/>
+      <c r="E1007" s="32"/>
+    </row>
+    <row r="1008" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C1008" s="31"/>
+      <c r="D1008" s="31"/>
+      <c r="E1008" s="32"/>
+    </row>
+    <row r="1009" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C1009" s="31"/>
+      <c r="D1009" s="31"/>
+      <c r="E1009" s="32"/>
+    </row>
+    <row r="1010" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C1010" s="31"/>
+      <c r="D1010" s="31"/>
+      <c r="E1010" s="32"/>
+    </row>
+    <row r="1011" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C1011" s="31"/>
+      <c r="D1011" s="31"/>
+      <c r="E1011" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>